<commit_message>
Planeacion Actualizada y primera version de la Documentacion
</commit_message>
<xml_diff>
--- a/doc/Planeacion.xlsx
+++ b/doc/Planeacion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaby__000\Desktop\Maestria\Sistemas Distribuidos\proyecto\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaby__000\Desktop\Maestria\Sistemas Distribuidos\proyecto\Bluetooth_Game\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma de Actividades" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Gabriela Márquez Quezada</author>
   </authors>
   <commentList>
-    <comment ref="A68" authorId="0" shapeId="0">
+    <comment ref="A71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="151">
   <si>
     <t>Nombre de tarea</t>
   </si>
@@ -392,9 +392,6 @@
     <t xml:space="preserve">      Modulo de Comunicación Distribuida</t>
   </si>
   <si>
-    <t>47CC</t>
-  </si>
-  <si>
     <t xml:space="preserve">         Implementación de código que para lógica del Juego</t>
   </si>
   <si>
@@ -455,40 +452,67 @@
     <t xml:space="preserve">   Control del Código en Git</t>
   </si>
   <si>
-    <t>Gabriela Marquez Quezada,Arturo López González</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Planteamiento de Casos de Prueba con diagramas</t>
-  </si>
-  <si>
-    <t>20 días</t>
-  </si>
-  <si>
-    <t>sáb 26/03/16</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Diagrama de Arquitectura del Sistema Distribuido</t>
   </si>
   <si>
-    <t>52,54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Integración de Código de Módulos de Comunicación en proyecto de GUI-GameEngine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Creación de funciones y adecuación de código del Game Engine para integración de módulos de comunicación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Corrección de código de GUI para optimización de espacio de memoria</t>
-  </si>
-  <si>
     <t>71 días</t>
   </si>
   <si>
-    <t xml:space="preserve">   Realización de Diagramas de Flujo del Cada Módulo</t>
-  </si>
-  <si>
     <t>ATRASADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Creacion de funciones para interfaz con modulos de comunicacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Corrección de codigo de GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Integración de Codigo de Modulos de Comunicación en proyecto de GUI-GameEngine</t>
+  </si>
+  <si>
+    <t>Alejandro Susarrey,Gabriela Marquez Quezada,Héctor Valle,Luis Angel Muñoz Mitre</t>
+  </si>
+  <si>
+    <t>6.42 días</t>
+  </si>
+  <si>
+    <t>mié 27/04/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Implementacion de Manejo de Excepciones</t>
+  </si>
+  <si>
+    <t>6 días</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Realizacion de Pruebas de acuerdo a los Casos de uso definidos</t>
+  </si>
+  <si>
+    <t>Gabriela Marquez Quezada,Héctor Valle,Luis Angel Muñoz Mitre,Jose Luis Sampayo</t>
+  </si>
+  <si>
+    <t>44CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Planteamiento de Estructura de la Documentacion</t>
+  </si>
+  <si>
+    <t>sáb 09/04/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Planteamiento de Casos de Uso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Realizacion de Documentacion de acuerdo a la estructura planteada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Documentacion de Casos de Prueba</t>
+  </si>
+  <si>
+    <t>54, 58</t>
+  </si>
+  <si>
+    <t>52,56</t>
   </si>
 </sst>
 </file>
@@ -688,7 +712,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -845,22 +869,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1093,26 +1106,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1251,34 +1258,34 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:colOff>70468</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>706757</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>52388</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 118"/>
+        <xdr:cNvPr id="2127" name="Group 79"/>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="99060" y="2255520"/>
-          <a:ext cx="17303117" cy="1637348"/>
-          <a:chOff x="-79" y="-112"/>
-          <a:chExt cx="1817" cy="191"/>
+          <a:off x="70468" y="2659380"/>
+          <a:ext cx="22195172" cy="1276350"/>
+          <a:chOff x="-48" y="-56"/>
+          <a:chExt cx="1797" cy="134"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 156"/>
+          <xdr:cNvPr id="2164" name="Rectangle 116"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -1286,13 +1293,13 @@
         <xdr:spPr bwMode="auto">
           <a:xfrm>
             <a:off x="18" y="0"/>
-            <a:ext cx="1635" cy="78"/>
+            <a:ext cx="1645" cy="78"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:schemeClr val="tx1"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:ln w="1">
             <a:solidFill>
@@ -1306,15 +1313,15 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 155" descr="jue 28/01/16"/>
+          <xdr:cNvPr id="2163" name="Rectangle 115" descr="jue 28/01/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="-79" y="-3"/>
-            <a:ext cx="91" cy="38"/>
+            <a:off x="-48" y="7"/>
+            <a:ext cx="60" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -1387,15 +1394,15 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 154" descr="vie 29/04/16"/>
+          <xdr:cNvPr id="2162" name="Rectangle 114" descr="jue 28/04/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1659" y="-3"/>
-            <a:ext cx="79" cy="38"/>
+            <a:off x="1669" y="-3"/>
+            <a:ext cx="80" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -1468,14 +1475,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Rectangle 153" descr="31 ene '16"/>
+          <xdr:cNvPr id="2161" name="Rectangle 113" descr="31 ene '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="72" y="-19"/>
+            <a:off x="71" y="-19"/>
             <a:ext cx="66" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -1527,14 +1534,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="Freeform 152"/>
+          <xdr:cNvPr id="2160" name="Freeform 112"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="72" y="-14"/>
+            <a:off x="71" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -1580,14 +1587,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Rectangle 151" descr="07 feb '16"/>
+          <xdr:cNvPr id="2159" name="Rectangle 111" descr="07 feb '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="196" y="-19"/>
+            <a:off x="197" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -1639,14 +1646,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Freeform 150"/>
+          <xdr:cNvPr id="2158" name="Freeform 110"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="196" y="-14"/>
+            <a:off x="197" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -1692,14 +1699,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Rectangle 149" descr="14 feb '16"/>
+          <xdr:cNvPr id="2157" name="Rectangle 109" descr="14 feb '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="320" y="-19"/>
+            <a:off x="322" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -1751,14 +1758,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="Freeform 148"/>
+          <xdr:cNvPr id="2156" name="Freeform 108"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="320" y="-14"/>
+            <a:off x="322" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -1804,14 +1811,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="Rectangle 147" descr="21 feb '16"/>
+          <xdr:cNvPr id="2155" name="Rectangle 107" descr="21 feb '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="445" y="-19"/>
+            <a:off x="447" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -1863,14 +1870,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="Freeform 146"/>
+          <xdr:cNvPr id="2154" name="Freeform 106"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="445" y="-14"/>
+            <a:off x="447" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -1916,14 +1923,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Rectangle 145" descr="28 feb '16"/>
+          <xdr:cNvPr id="2153" name="Rectangle 105" descr="28 feb '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="569" y="-19"/>
+            <a:off x="572" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -1975,14 +1982,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="Freeform 144"/>
+          <xdr:cNvPr id="2152" name="Freeform 104"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="569" y="-14"/>
+            <a:off x="572" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2028,14 +2035,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="Rectangle 143" descr="06 mar '16"/>
+          <xdr:cNvPr id="2151" name="Rectangle 103" descr="06 mar '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="694" y="-19"/>
+            <a:off x="697" y="-19"/>
             <a:ext cx="67" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2087,14 +2094,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="17" name="Freeform 142"/>
+          <xdr:cNvPr id="2150" name="Freeform 102"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="694" y="-14"/>
+            <a:off x="697" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2140,14 +2147,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="18" name="Rectangle 141" descr="13 mar '16"/>
+          <xdr:cNvPr id="2149" name="Rectangle 101" descr="13 mar '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="818" y="-19"/>
+            <a:off x="823" y="-19"/>
             <a:ext cx="67" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2199,14 +2206,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="19" name="Freeform 140"/>
+          <xdr:cNvPr id="2148" name="Freeform 100"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="818" y="-14"/>
+            <a:off x="823" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2252,14 +2259,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="Rectangle 139" descr="20 mar '16"/>
+          <xdr:cNvPr id="2147" name="Rectangle 99" descr="20 mar '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="942" y="-19"/>
+            <a:off x="948" y="-19"/>
             <a:ext cx="67" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2311,14 +2318,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="21" name="Freeform 138"/>
+          <xdr:cNvPr id="2146" name="Freeform 98"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="942" y="-14"/>
+            <a:off x="948" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2364,14 +2371,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="22" name="Rectangle 137" descr="27 mar '16"/>
+          <xdr:cNvPr id="2145" name="Rectangle 97" descr="27 mar '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1067" y="-19"/>
+            <a:off x="1073" y="-19"/>
             <a:ext cx="67" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2423,14 +2430,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="23" name="Freeform 136"/>
+          <xdr:cNvPr id="2144" name="Freeform 96"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1067" y="-14"/>
+            <a:off x="1073" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2476,14 +2483,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="24" name="Rectangle 135" descr="03 abr '16"/>
+          <xdr:cNvPr id="2143" name="Rectangle 95" descr="03 abr '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1191" y="-19"/>
+            <a:off x="1198" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2535,14 +2542,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="25" name="Freeform 134"/>
+          <xdr:cNvPr id="2142" name="Freeform 94"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1191" y="-14"/>
+            <a:off x="1198" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2588,14 +2595,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="26" name="Rectangle 133" descr="10 abr '16"/>
+          <xdr:cNvPr id="2141" name="Rectangle 93" descr="10 abr '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1316" y="-19"/>
+            <a:off x="1323" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2647,14 +2654,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="27" name="Freeform 132"/>
+          <xdr:cNvPr id="2140" name="Freeform 92"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1316" y="-14"/>
+            <a:off x="1323" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2700,14 +2707,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="28" name="Rectangle 131" descr="17 abr '16"/>
+          <xdr:cNvPr id="2139" name="Rectangle 91" descr="17 abr '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1440" y="-19"/>
+            <a:off x="1449" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2759,14 +2766,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Freeform 130"/>
+          <xdr:cNvPr id="2138" name="Freeform 90"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1440" y="-14"/>
+            <a:off x="1449" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2812,14 +2819,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="30" name="Rectangle 129" descr="24 abr '16"/>
+          <xdr:cNvPr id="2137" name="Rectangle 89" descr="24 abr '16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1564" y="-19"/>
+            <a:off x="1574" y="-19"/>
             <a:ext cx="63" cy="19"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2871,14 +2878,14 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="31" name="Freeform 128"/>
+          <xdr:cNvPr id="2136" name="Freeform 88"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1564" y="-14"/>
+            <a:off x="1574" y="-14"/>
             <a:ext cx="0" cy="14"/>
           </a:xfrm>
           <a:custGeom>
@@ -2924,7 +2931,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="32" name="Rectangle 127" descr="Exploracion&#10;jue 28/01/16 - jue 18/02/16"/>
+          <xdr:cNvPr id="2135" name="Rectangle 87" descr="Exploracion&#10;jue 28/01/16 - jue 18/02/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -2932,7 +2939,7 @@
         <xdr:spPr bwMode="auto">
           <a:xfrm>
             <a:off x="19" y="1"/>
-            <a:ext cx="390" cy="38"/>
+            <a:ext cx="392" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3000,15 +3007,15 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="33" name="Rectangle 126" descr="Inicializacion&#10;jue 11/02/16 - jue 03/03/16"/>
+          <xdr:cNvPr id="2134" name="Rectangle 86" descr="Inicializacion&#10;jue 11/02/16 - jue 03/03/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="268" y="40"/>
-            <a:ext cx="372" cy="38"/>
+            <a:off x="269" y="40"/>
+            <a:ext cx="375" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3076,37 +3083,22 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="34" name="Rectangle 125" descr="Produccion&#10;vie 19/02/16 - mié 06/04/16"/>
+          <xdr:cNvPr id="2133" name="Rectangle 85" descr="Produccion&#10;vie 19/02/16 - mié 06/04/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="410" y="1"/>
-            <a:ext cx="834" cy="38"/>
+            <a:off x="412" y="1"/>
+            <a:ext cx="840" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-          <a:gradFill flip="none" rotWithShape="1">
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:srgbClr val="00B050"/>
-              </a:gs>
-              <a:gs pos="13000">
-                <a:srgbClr val="00B050"/>
-              </a:gs>
-              <a:gs pos="78000">
-                <a:srgbClr val="00B050"/>
-              </a:gs>
-              <a:gs pos="90000">
-                <a:schemeClr val="accent4"/>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="0" scaled="1"/>
-            <a:tileRect/>
-          </a:gradFill>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
@@ -3167,30 +3159,22 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="35" name="Rectangle 124" descr="Estabilización&#10;mié 06/04/16 - sáb 16/04/16"/>
+          <xdr:cNvPr id="2132" name="Rectangle 84" descr="Estabilización&#10;mié 06/04/16 - jue 21/04/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1245" y="1"/>
-            <a:ext cx="177" cy="38"/>
+            <a:off x="1253" y="1"/>
+            <a:ext cx="267" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-          <a:gradFill>
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:srgbClr val="00B050"/>
-              </a:gs>
-              <a:gs pos="22000">
-                <a:srgbClr val="FFC000"/>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="0" scaled="1"/>
-          </a:gradFill>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
@@ -3244,32 +3228,32 @@
                 <a:latin typeface="Segoe UI"/>
                 <a:cs typeface="Segoe UI"/>
               </a:rPr>
-              <a:t>mié 06/04/16 - sáb 16/04/16</a:t>
+              <a:t>mié 06/04/16 - jue 21/04/16</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="36" name="Rectangle 123" descr="Documentacion&#10;mié 06/04/16 - vie 29/04/16"/>
+          <xdr:cNvPr id="2131" name="Rectangle 83" descr="Documentacion&#10;mié 06/04/16 - mié 27/04/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1245" y="40"/>
-            <a:ext cx="356" cy="38"/>
+            <a:off x="1253" y="40"/>
+            <a:ext cx="374" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
           <a:gradFill>
             <a:gsLst>
-              <a:gs pos="0">
+              <a:gs pos="38000">
                 <a:srgbClr val="00B050"/>
               </a:gs>
-              <a:gs pos="8000">
+              <a:gs pos="57000">
                 <a:srgbClr val="FFC000"/>
               </a:gs>
             </a:gsLst>
@@ -3328,53 +3312,37 @@
                 <a:latin typeface="Segoe UI"/>
                 <a:cs typeface="Segoe UI"/>
               </a:rPr>
-              <a:t>mié 06/04/16 - </a:t>
+              <a:t>mié 06/04/16 - mié 27/04/16</a:t>
             </a:r>
-            <a:r>
-              <a:rPr kumimoji="0" lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="444444"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:uLnTx/>
-                <a:uFillTx/>
-                <a:latin typeface="Segoe UI"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Segoe UI"/>
-              </a:rPr>
-              <a:t>mar 26/04/16</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="444444"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI"/>
-              <a:cs typeface="Segoe UI"/>
-            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="37" name="Rectangle 122" descr="Pruebas y Correccion&#10;sáb 16/04/16 - mar 26/04/16"/>
+          <xdr:cNvPr id="2130" name="Rectangle 82" descr="Pruebas y Correccion&#10;jue 21/04/16 - mié 27/04/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1423" y="1"/>
-            <a:ext cx="177" cy="38"/>
+            <a:off x="1521" y="1"/>
+            <a:ext cx="124" cy="38"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="7000">
+                <a:srgbClr val="00B050"/>
+              </a:gs>
+              <a:gs pos="42000">
+                <a:srgbClr val="FFC000"/>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="0" scaled="1"/>
+          </a:gradFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
@@ -3428,143 +3396,21 @@
                 <a:latin typeface="Segoe UI"/>
                 <a:cs typeface="Segoe UI"/>
               </a:rPr>
-              <a:t>sáb 16/04/16 - mar 26/04/16</a:t>
+              <a:t>jue 21/04/16 - mié 27/04/16</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="38" name="AutoShape 121"/>
+          <xdr:cNvPr id="2129" name="Freeform 81"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="-79" y="-112"/>
-            <a:ext cx="1817" cy="191"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="T0" fmla="+- 0 1600 -79"/>
-              <a:gd name="T1" fmla="*/ T0 w 1817"/>
-              <a:gd name="T2" fmla="+- 0 0 -112"/>
-              <a:gd name="T3" fmla="*/ 0 h 191"/>
-              <a:gd name="T4" fmla="+- 0 1600 -79"/>
-              <a:gd name="T5" fmla="*/ T4 w 1817"/>
-              <a:gd name="T6" fmla="+- 0 -28 -112"/>
-              <a:gd name="T7" fmla="*/ -28 h 191"/>
-              <a:gd name="T8" fmla="+- 0 1600 -79"/>
-              <a:gd name="T9" fmla="*/ T8 w 1817"/>
-              <a:gd name="T10" fmla="+- 0 -28 -112"/>
-              <a:gd name="T11" fmla="*/ -28 h 191"/>
-              <a:gd name="T12" fmla="+- 0 1604 -79"/>
-              <a:gd name="T13" fmla="*/ T12 w 1817"/>
-              <a:gd name="T14" fmla="+- 0 -32 -112"/>
-              <a:gd name="T15" fmla="*/ -32 h 191"/>
-              <a:gd name="T16" fmla="+- 0 1649 -79"/>
-              <a:gd name="T17" fmla="*/ T16 w 1817"/>
-              <a:gd name="T18" fmla="+- 0 -32 -112"/>
-              <a:gd name="T19" fmla="*/ -32 h 191"/>
-              <a:gd name="T20" fmla="+- 0 1649 -79"/>
-              <a:gd name="T21" fmla="*/ T20 w 1817"/>
-              <a:gd name="T22" fmla="+- 0 -32 -112"/>
-              <a:gd name="T23" fmla="*/ -32 h 191"/>
-              <a:gd name="T24" fmla="+- 0 1653 -79"/>
-              <a:gd name="T25" fmla="*/ T24 w 1817"/>
-              <a:gd name="T26" fmla="+- 0 -28 -112"/>
-              <a:gd name="T27" fmla="*/ -28 h 191"/>
-              <a:gd name="T28" fmla="+- 0 1653 -79"/>
-              <a:gd name="T29" fmla="*/ T28 w 1817"/>
-              <a:gd name="T30" fmla="+- 0 0 -112"/>
-              <a:gd name="T31" fmla="*/ 0 h 191"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="T1" y="T3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T5" y="T7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T9" y="T11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T13" y="T15"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T17" y="T19"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T21" y="T23"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T25" y="T27"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T29" y="T31"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="0" t="0" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="1817" h="191">
-                <a:moveTo>
-                  <a:pt x="1679" y="112"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="1679" y="84"/>
-                </a:lnTo>
-                <a:moveTo>
-                  <a:pt x="1679" y="84"/>
-                </a:moveTo>
-                <a:cubicBezTo>
-                  <a:pt x="1679" y="81"/>
-                  <a:pt x="1680" y="80"/>
-                  <a:pt x="1683" y="80"/>
-                </a:cubicBezTo>
-                <a:lnTo>
-                  <a:pt x="1728" y="80"/>
-                </a:lnTo>
-                <a:moveTo>
-                  <a:pt x="1728" y="80"/>
-                </a:moveTo>
-                <a:cubicBezTo>
-                  <a:pt x="1730" y="80"/>
-                  <a:pt x="1732" y="81"/>
-                  <a:pt x="1732" y="84"/>
-                </a:cubicBezTo>
-                <a:lnTo>
-                  <a:pt x="1732" y="112"/>
-                </a:lnTo>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFFFFF"/>
-          </a:solidFill>
-          <a:ln w="1">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:round/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="39" name="Freeform 120"/>
-          <xdr:cNvSpPr>
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1626" y="-55"/>
+            <a:off x="1654" y="-23"/>
             <a:ext cx="0" cy="23"/>
           </a:xfrm>
           <a:custGeom>
@@ -3610,15 +3456,15 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="40" name="Rectangle 119" descr="Producto Final&#10;mar 26/04/16 - vie 29/04/16"/>
+          <xdr:cNvPr id="2128" name="Rectangle 80" descr="Producto Final&#10;mié 27/04/16 - jue 28/04/16"/>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="1569" y="-111"/>
-            <a:ext cx="115" cy="56"/>
+            <a:off x="1611" y="-56"/>
+            <a:ext cx="115" cy="34"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3684,7 +3530,7 @@
                 <a:latin typeface="Segoe UI"/>
                 <a:cs typeface="Segoe UI"/>
               </a:rPr>
-              <a:t>mar 26/04/16 - jue 28/04/16</a:t>
+              <a:t>mié 27/04/16 - jue 28/04/16</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -3958,13 +3804,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE69"/>
+  <dimension ref="A1:AE72"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="34.44140625" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -4561,10 +4407,10 @@
       <c r="G15" s="32"/>
       <c r="H15" s="5">
         <f>AVERAGE(H16,H32)</f>
-        <v>0.93125000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="13.8" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4587,7 +4433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4610,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="86.4" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="86.4" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4634,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.8" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="28.8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4660,7 +4506,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="43.2" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="43.2" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4684,7 +4530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4709,7 +4555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.8" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="28.8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4735,7 +4581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4759,7 +4605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.8" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="28.8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -4783,7 +4629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -4806,7 +4652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="28.8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -4832,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="43.2" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="43.2" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4858,7 +4704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -4882,12 +4728,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="55" t="s">
         <v>85</v>
@@ -4905,7 +4751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="28.8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -4929,7 +4775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="28.8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -4953,7 +4799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -4961,7 +4807,7 @@
         <v>89</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" s="68" t="s">
         <v>64</v>
@@ -4973,10 +4819,10 @@
       <c r="G32" s="8"/>
       <c r="H32" s="25">
         <f>AVERAGE(H33,H37,H40,H42)</f>
-        <v>0.86250000000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5001,7 +4847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="28.8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5027,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5052,12 +4898,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="28.8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>87</v>
@@ -5078,7 +4924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="16.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="16.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -5086,7 +4932,7 @@
         <v>108</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D37" s="77" t="s">
         <v>64</v>
@@ -5103,12 +4949,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="28.8" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>38</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>18</v>
@@ -5127,12 +4973,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="43.2" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="43.2" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>39</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>87</v>
@@ -5153,7 +4999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="28.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>41</v>
       </c>
@@ -5175,34 +5021,34 @@
       <c r="G40" s="59"/>
       <c r="H40" s="23">
         <f>AVERAGE(H41:H41)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="57.6" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="57.6" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>42</v>
       </c>
-      <c r="B41" s="83" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="83" t="s">
+      <c r="B41" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="84" t="s">
+      <c r="D41" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83" t="s">
+      <c r="F41" s="36"/>
+      <c r="G41" s="36" t="s">
         <v>66</v>
       </c>
       <c r="H41" s="23">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="28.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>44</v>
       </c>
@@ -5210,7 +5056,7 @@
         <v>91</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D42" s="76" t="s">
         <v>64</v>
@@ -5222,10 +5068,10 @@
       <c r="G42" s="53"/>
       <c r="H42" s="26">
         <f>AVERAGE(H43:H44)</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="28.8" outlineLevel="3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="28.8" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>45</v>
       </c>
@@ -5250,31 +5096,31 @@
       </c>
       <c r="I43" s="81"/>
     </row>
-    <row r="44" spans="1:9" ht="72" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="72" hidden="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>46</v>
       </c>
-      <c r="B44" s="85" t="s">
+      <c r="B44" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="87" t="s">
+      <c r="D44" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="87" t="s">
+      <c r="E44" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="86"/>
-      <c r="G44" s="83" t="s">
+      <c r="F44" s="84"/>
+      <c r="G44" s="36" t="s">
         <v>93</v>
       </c>
       <c r="H44" s="23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>47</v>
       </c>
@@ -5282,29 +5128,29 @@
         <v>32</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D45" s="69" t="s">
         <v>42</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="F45" s="4">
         <v>14</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="5">
-        <f>AVERAGE(H46:H49)</f>
-        <v>0.13250000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
+        <f>AVERAGE(H46,H49)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="28.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>48</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>85</v>
@@ -5313,7 +5159,7 @@
         <v>42</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F46" s="22">
         <v>31</v>
@@ -5322,15 +5168,15 @@
         <v>55</v>
       </c>
       <c r="H46" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>49</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>43</v>
@@ -5342,47 +5188,47 @@
         <v>44</v>
       </c>
       <c r="F47" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G47" s="21" t="s">
         <v>55</v>
       </c>
       <c r="H47" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="43.2" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>50</v>
       </c>
-      <c r="B48" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="21" t="s">
+      <c r="B48" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="22">
+      <c r="E48" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F48" s="36">
         <v>31</v>
       </c>
-      <c r="G48" s="21" t="s">
-        <v>129</v>
+      <c r="G48" s="36" t="s">
+        <v>128</v>
       </c>
       <c r="H48" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="72" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="57.6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>51</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C49" s="21" t="s">
         <v>43</v>
@@ -5395,13 +5241,13 @@
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="21" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="H49" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>52</v>
       </c>
@@ -5409,215 +5255,311 @@
         <v>33</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="D50" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="E50" s="69" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="F50" s="4">
         <v>47</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="72" outlineLevel="1" x14ac:dyDescent="0.3">
+        <f>AVERAGE(H51,H53)</f>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>53</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H51" s="82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="H51" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>54</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D52" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G52" s="4"/>
+      <c r="B52" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" s="22"/>
+      <c r="G52" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="H52" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="57.6" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>55</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F53" s="22">
-        <v>31</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F53" s="22"/>
       <c r="G53" s="21" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="H53" s="5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>56</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D54" s="21" t="s">
+      <c r="B54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="E54" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="22">
-        <v>31</v>
-      </c>
-      <c r="G54" s="21" t="s">
-        <v>54</v>
-      </c>
+      <c r="E54" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="4"/>
       <c r="H54" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <f>AVERAGE(H55,H59)</f>
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>57</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>42</v>
+        <v>145</v>
       </c>
       <c r="E55" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F55" s="22">
-        <v>31</v>
-      </c>
+      <c r="F55" s="22"/>
       <c r="G55" s="21" t="s">
         <v>13</v>
       </c>
       <c r="H55" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>58</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="22"/>
+      <c r="G56" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
+        <v>59</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A58" s="3">
+        <v>60</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F58" s="22">
+        <v>57</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
+        <v>61</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F59" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="G59" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H59" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
+        <v>62</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="69" t="s">
+      <c r="C60" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E60" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="F56" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G56" s="4"/>
-      <c r="H56" s="5">
+      <c r="F60" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="12" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="14" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="15" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D64" s="20"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16" t="s">
+      <c r="D68" s="20"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="17" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="41" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="41" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="88" t="s">
-        <v>142</v>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="82" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H32 H34:H56">
+  <conditionalFormatting sqref="H2:H32 H34:H60">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="between">
       <formula>0.01</formula>
       <formula>0.99</formula>
@@ -5644,7 +5586,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H10 H35 H45" formulaRange="1"/>
+    <ignoredError sqref="H10 H35" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -5654,8 +5596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5687,13 +5629,13 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" s="63" t="s">
         <v>100</v>
@@ -5703,12 +5645,12 @@
       </c>
       <c r="F2" s="61">
         <f>AVERAGE(F3:F11)</f>
-        <v>0.77777777777777779</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="65" t="s">
         <v>41</v>
@@ -5726,7 +5668,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="65" t="s">
         <v>41</v>
@@ -5744,7 +5686,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="65" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="65" t="s">
         <v>41</v>
@@ -5762,7 +5704,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="65" t="s">
         <v>41</v>
@@ -5780,7 +5722,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="65" t="s">
         <v>41</v>
@@ -5798,7 +5740,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="65" t="s">
         <v>41</v>
@@ -5816,7 +5758,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="65" t="s">
         <v>41</v>
@@ -5834,7 +5776,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="65" t="s">
         <v>41</v>
@@ -5847,12 +5789,12 @@
       </c>
       <c r="E10" s="66"/>
       <c r="F10" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" s="65" t="s">
         <v>41</v>
@@ -5865,7 +5807,7 @@
       </c>
       <c r="E11" s="66"/>
       <c r="F11" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -5962,7 +5904,6 @@
       <c r="G23" s="48"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="47"/>
       <c r="B24" s="47"/>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>

</xml_diff>